<commit_message>
Přidána dokumentaci. Vytvořena třída shrnující standardní odpovědi. Čištění a přejmenování Vytvořen timeline na 2 další týdny. StandardResponseMessage.cs sjednocuje odpovědi serveru. Vytvořen Util.cs
</commit_message>
<xml_diff>
--- a/timeline/1M Project Timeline.xlsx
+++ b/timeline/1M Project Timeline.xlsx
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -169,6 +169,18 @@
   </si>
   <si>
     <t>Daemon tasky</t>
+  </si>
+  <si>
+    <t>HTTPS</t>
+  </si>
+  <si>
+    <t>Návrh admin app</t>
+  </si>
+  <si>
+    <t>Základní error reporting</t>
+  </si>
+  <si>
+    <t>Bug fixy &amp; Zlepšení</t>
   </si>
 </sst>
 </file>
@@ -231,13 +243,6 @@
       <scheme val="major"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
@@ -250,8 +255,14 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -296,25 +307,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF7030A0"/>
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -479,6 +484,24 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="10">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -496,24 +519,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -766,8 +771,8 @@
   </sheetPr>
   <dimension ref="B1:AF27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O12" sqref="O12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W20" sqref="W20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -781,91 +786,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="31">
         <v>43143</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="26"/>
-      <c r="G4" s="26"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="26"/>
-      <c r="J4" s="24" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="26" t="s">
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="26"/>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="24" t="s">
+      <c r="R4" s="32"/>
+      <c r="S4" s="32"/>
+      <c r="T4" s="32"/>
+      <c r="U4" s="32"/>
+      <c r="V4" s="32"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="24"/>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24"/>
-      <c r="AB4" s="24"/>
-      <c r="AC4" s="24"/>
-      <c r="AD4" s="24"/>
-      <c r="AE4" s="21" t="s">
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="27" t="s">
         <v>7</v>
       </c>
       <c r="AF4" t="s">
@@ -986,7 +991,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE5" s="21"/>
+      <c r="AE5" s="27"/>
       <c r="AF5" t="s">
         <v>6</v>
       </c>
@@ -1105,7 +1110,7 @@
         <f t="shared" si="1"/>
         <v>sun</v>
       </c>
-      <c r="AE6" s="21"/>
+      <c r="AE6" s="27"/>
     </row>
     <row r="7" spans="2:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -1223,19 +1228,19 @@
         <f t="shared" ref="AD7" si="5">AC7+1</f>
         <v>43170</v>
       </c>
-      <c r="AE7" s="22"/>
+      <c r="AE7" s="28"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
       <c r="H8" s="6"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
@@ -1265,13 +1270,13 @@
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
       <c r="H9" s="6"/>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
@@ -1306,15 +1311,14 @@
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
       <c r="G10" s="5"/>
-      <c r="H10" s="29" t="s">
+      <c r="I10" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="29"/>
-      <c r="J10" s="29"/>
-      <c r="K10" s="29"/>
-      <c r="L10" s="29"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="29"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="24"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="5"/>
@@ -1342,15 +1346,15 @@
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="30" t="s">
+      <c r="H11" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="30"/>
-      <c r="J11" s="30"/>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="30"/>
-      <c r="N11" s="30"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="5"/>
@@ -1378,15 +1382,15 @@
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="31" t="s">
+      <c r="H12" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31"/>
-      <c r="K12" s="31"/>
-      <c r="L12" s="31"/>
-      <c r="M12" s="31"/>
-      <c r="N12" s="31"/>
+      <c r="I12" s="26"/>
+      <c r="J12" s="26"/>
+      <c r="K12" s="26"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="26"/>
       <c r="O12" s="5"/>
       <c r="P12" s="6"/>
       <c r="Q12" s="5"/>
@@ -1405,7 +1409,7 @@
       <c r="AD12" s="6"/>
       <c r="AE12" s="20"/>
     </row>
-    <row r="13" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:32" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
         <v>18</v>
       </c>
@@ -1418,13 +1422,13 @@
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="30" t="s">
+      <c r="L13" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="30"/>
-      <c r="N13" s="30"/>
-      <c r="O13" s="30"/>
-      <c r="P13" s="30"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="6"/>
       <c r="S13" s="5"/>
@@ -1452,18 +1456,18 @@
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-      <c r="M14" s="32"/>
-      <c r="N14" s="32"/>
-      <c r="O14" s="32"/>
-      <c r="P14" s="32"/>
-      <c r="Q14" s="32"/>
-      <c r="R14" s="32"/>
-      <c r="S14" s="32"/>
+      <c r="K14" s="25"/>
+      <c r="L14" s="25"/>
+      <c r="M14" s="25"/>
+      <c r="N14" s="25"/>
+      <c r="O14" s="25"/>
+      <c r="P14" s="25"/>
+      <c r="Q14" s="25"/>
+      <c r="R14" s="25"/>
+      <c r="S14" s="25"/>
       <c r="T14" s="6"/>
       <c r="U14" s="5"/>
       <c r="V14" s="6"/>
@@ -1478,7 +1482,9 @@
       <c r="AE14" s="20"/>
     </row>
     <row r="15" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="19"/>
+      <c r="B15" s="19" t="s">
+        <v>20</v>
+      </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
       <c r="E15" s="5"/>
@@ -1494,12 +1500,14 @@
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="6"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="6"/>
-      <c r="W15" s="5"/>
+      <c r="R15" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="22"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="5"/>
       <c r="Z15" s="6"/>
@@ -1510,25 +1518,31 @@
       <c r="AE15" s="20"/>
     </row>
     <row r="16" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="19"/>
+      <c r="B16" s="19" t="s">
+        <v>21</v>
+      </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="6"/>
+      <c r="H16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
       <c r="M16" s="5"/>
       <c r="N16" s="6"/>
       <c r="O16" s="5"/>
       <c r="P16" s="6"/>
-      <c r="Q16" s="5"/>
-      <c r="R16" s="6"/>
-      <c r="S16" s="5"/>
-      <c r="T16" s="6"/>
+      <c r="Q16" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
+      <c r="T16" s="21"/>
       <c r="U16" s="5"/>
       <c r="V16" s="6"/>
       <c r="W16" s="5"/>
@@ -1541,8 +1555,10 @@
       <c r="AD16" s="6"/>
       <c r="AE16" s="20"/>
     </row>
-    <row r="17" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="19"/>
+    <row r="17" spans="2:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="19" t="s">
+        <v>22</v>
+      </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
       <c r="E17" s="5"/>
@@ -1553,12 +1569,14 @@
       <c r="J17" s="6"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="5"/>
-      <c r="N17" s="6"/>
-      <c r="O17" s="5"/>
-      <c r="P17" s="6"/>
-      <c r="Q17" s="5"/>
-      <c r="R17" s="6"/>
+      <c r="M17" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="N17" s="26"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="26"/>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="26"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
       <c r="U17" s="5"/>
@@ -1574,7 +1592,9 @@
       <c r="AE17" s="20"/>
     </row>
     <row r="18" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="19"/>
+      <c r="B18" s="19" t="s">
+        <v>23</v>
+      </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
       <c r="E18" s="5"/>
@@ -1592,10 +1612,12 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="6"/>
       <c r="S18" s="5"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="5"/>
+      <c r="T18" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="U18" s="25"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="25"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="6"/>
@@ -1894,12 +1916,7 @@
       <c r="AE27" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="J14:S14"/>
-    <mergeCell ref="H10:N10"/>
-    <mergeCell ref="H11:N11"/>
-    <mergeCell ref="H12:N12"/>
+  <mergeCells count="19">
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="AE4:AE7"/>
@@ -1909,6 +1926,16 @@
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="J4:P4"/>
     <mergeCell ref="Q4:W4"/>
+    <mergeCell ref="R15:V15"/>
+    <mergeCell ref="Q16:S16"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="J14:S14"/>
+    <mergeCell ref="H11:N11"/>
+    <mergeCell ref="H12:N12"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="0" priority="1">

</xml_diff>

<commit_message>
Vytvořena nová dokumentace.Vytvořeny message pro komunikaci s DB. Updatovaná timelina
</commit_message>
<xml_diff>
--- a/timeline/1M Project Timeline.xlsx
+++ b/timeline/1M Project Timeline.xlsx
@@ -104,12 +104,85 @@
         </r>
       </text>
     </comment>
+    <comment ref="H12" authorId="0" shapeId="0" xr:uid="{56319CBC-525B-4AFC-9841-8BC401B06261}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>lukx:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Prodlouženo</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AE13" authorId="0" shapeId="0" xr:uid="{F7C1B304-9226-4C83-875A-82D396B247D1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>lukx:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Předáno Rambovi.
+Druhy backapů byli přidány do DB</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="0" shapeId="0" xr:uid="{FE1D2AA7-EA35-473E-9EDB-FAD401627DB4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>lukx:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Useru, Daemonů, a DaemonPresharedKey</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="31">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -181,6 +254,27 @@
   </si>
   <si>
     <t>Bug fixy &amp; Zlepšení</t>
+  </si>
+  <si>
+    <t>Admin přidání znova …</t>
+  </si>
+  <si>
+    <t>Dokončeno</t>
+  </si>
+  <si>
+    <t>Nezačnuto</t>
+  </si>
+  <si>
+    <t>Probíha</t>
+  </si>
+  <si>
+    <t>Odloženo</t>
+  </si>
+  <si>
+    <t>Jiné</t>
+  </si>
+  <si>
+    <t>Přeloženo</t>
   </si>
 </sst>
 </file>
@@ -191,7 +285,7 @@
     <numFmt numFmtId="164" formatCode="d"/>
     <numFmt numFmtId="165" formatCode="mmm"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1" tint="0.24994659260841701"/>
@@ -260,6 +354,19 @@
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="11">
@@ -484,41 +591,41 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="10">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -534,7 +641,43 @@
     <cellStyle name="Status" xfId="10" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
     <cellStyle name="Weekday" xfId="7" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="1" tint="4.9989318521683403E-2"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <color theme="1" tint="4.9989318521683403E-2"/>
@@ -771,8 +914,8 @@
   </sheetPr>
   <dimension ref="B1:AF27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V16" sqref="V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -786,91 +929,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="28">
         <v>43143</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="32" t="s">
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="30" t="s">
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="27" t="s">
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="27"/>
+      <c r="AE4" s="24" t="s">
         <v>7</v>
       </c>
       <c r="AF4" t="s">
@@ -991,7 +1134,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE5" s="27"/>
+      <c r="AE5" s="24"/>
       <c r="AF5" t="s">
         <v>6</v>
       </c>
@@ -1110,7 +1253,7 @@
         <f t="shared" si="1"/>
         <v>sun</v>
       </c>
-      <c r="AE6" s="27"/>
+      <c r="AE6" s="24"/>
     </row>
     <row r="7" spans="2:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -1228,19 +1371,19 @@
         <f t="shared" ref="AD7" si="5">AC7+1</f>
         <v>43170</v>
       </c>
-      <c r="AE7" s="28"/>
+      <c r="AE7" s="25"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
       <c r="H8" s="6"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
@@ -1264,7 +1407,9 @@
       <c r="AB8" s="6"/>
       <c r="AC8" s="5"/>
       <c r="AD8" s="6"/>
-      <c r="AE8" s="20"/>
+      <c r="AE8" s="32" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="9" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
@@ -1300,7 +1445,9 @@
       <c r="AB9" s="6"/>
       <c r="AC9" s="5"/>
       <c r="AD9" s="6"/>
-      <c r="AE9" s="20"/>
+      <c r="AE9" s="32" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="19" t="s">
@@ -1311,14 +1458,14 @@
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
       <c r="G10" s="5"/>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="24"/>
+      <c r="J10" s="30"/>
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="30"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="5"/>
@@ -1335,7 +1482,9 @@
       <c r="AB10" s="6"/>
       <c r="AC10" s="5"/>
       <c r="AD10" s="6"/>
-      <c r="AE10" s="20"/>
+      <c r="AE10" s="32" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="19" t="s">
@@ -1371,7 +1520,9 @@
       <c r="AB11" s="6"/>
       <c r="AC11" s="5"/>
       <c r="AD11" s="6"/>
-      <c r="AE11" s="20"/>
+      <c r="AE11" s="32" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="19" t="s">
@@ -1382,24 +1533,24 @@
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="5"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="5"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="5"/>
-      <c r="T12" s="6"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="6"/>
-      <c r="W12" s="5"/>
+      <c r="I12" s="31"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="31"/>
+      <c r="L12" s="31"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="31"/>
+      <c r="P12" s="31"/>
+      <c r="Q12" s="31"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="31"/>
+      <c r="T12" s="31"/>
+      <c r="U12" s="31"/>
+      <c r="V12" s="31"/>
+      <c r="W12" s="31"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="5"/>
       <c r="Z12" s="6"/>
@@ -1407,7 +1558,9 @@
       <c r="AB12" s="6"/>
       <c r="AC12" s="5"/>
       <c r="AD12" s="6"/>
-      <c r="AE12" s="20"/>
+      <c r="AE12" s="32" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="13" spans="2:32" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
@@ -1443,7 +1596,9 @@
       <c r="AB13" s="6"/>
       <c r="AC13" s="5"/>
       <c r="AD13" s="6"/>
-      <c r="AE13" s="20"/>
+      <c r="AE13" s="32" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
@@ -1456,18 +1611,18 @@
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="25" t="s">
+      <c r="J14" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="25"/>
-      <c r="L14" s="25"/>
-      <c r="M14" s="25"/>
-      <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
-      <c r="P14" s="25"/>
-      <c r="Q14" s="25"/>
-      <c r="R14" s="25"/>
-      <c r="S14" s="25"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="22"/>
+      <c r="N14" s="22"/>
+      <c r="O14" s="22"/>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="22"/>
       <c r="T14" s="6"/>
       <c r="U14" s="5"/>
       <c r="V14" s="6"/>
@@ -1479,7 +1634,9 @@
       <c r="AB14" s="6"/>
       <c r="AC14" s="5"/>
       <c r="AD14" s="6"/>
-      <c r="AE14" s="20"/>
+      <c r="AE14" s="32" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="15" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
@@ -1507,7 +1664,7 @@
       <c r="T15" s="23"/>
       <c r="U15" s="23"/>
       <c r="V15" s="23"/>
-      <c r="W15" s="22"/>
+      <c r="W15" s="21"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="5"/>
       <c r="Z15" s="6"/>
@@ -1515,7 +1672,9 @@
       <c r="AB15" s="6"/>
       <c r="AC15" s="5"/>
       <c r="AD15" s="6"/>
-      <c r="AE15" s="20"/>
+      <c r="AE15" s="32" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="16" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
@@ -1526,23 +1685,20 @@
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="30"/>
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
       <c r="M16" s="5"/>
       <c r="N16" s="6"/>
       <c r="O16" s="5"/>
       <c r="P16" s="6"/>
-      <c r="Q16" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="21"/>
+      <c r="Q16" s="5"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="6"/>
       <c r="U16" s="5"/>
       <c r="V16" s="6"/>
       <c r="W16" s="5"/>
@@ -1553,7 +1709,9 @@
       <c r="AB16" s="6"/>
       <c r="AC16" s="5"/>
       <c r="AD16" s="6"/>
-      <c r="AE16" s="20"/>
+      <c r="AE16" s="32" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="17" spans="2:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
@@ -1569,14 +1727,14 @@
       <c r="J17" s="6"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="26" t="s">
+      <c r="M17" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="31"/>
+      <c r="P17" s="31"/>
+      <c r="Q17" s="31"/>
+      <c r="R17" s="31"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
       <c r="U17" s="5"/>
@@ -1589,7 +1747,9 @@
       <c r="AB17" s="6"/>
       <c r="AC17" s="5"/>
       <c r="AD17" s="6"/>
-      <c r="AE17" s="20"/>
+      <c r="AE17" s="32" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="18" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
@@ -1612,12 +1772,12 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="6"/>
       <c r="S18" s="5"/>
-      <c r="T18" s="25" t="s">
+      <c r="T18" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="U18" s="25"/>
-      <c r="V18" s="25"/>
-      <c r="W18" s="25"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="6"/>
@@ -1625,10 +1785,14 @@
       <c r="AB18" s="6"/>
       <c r="AC18" s="5"/>
       <c r="AD18" s="6"/>
-      <c r="AE18" s="20"/>
+      <c r="AE18" s="32" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="19"/>
+      <c r="B19" s="19" t="s">
+        <v>24</v>
+      </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
       <c r="E19" s="5"/>
@@ -1643,13 +1807,15 @@
       <c r="N19" s="6"/>
       <c r="O19" s="5"/>
       <c r="P19" s="6"/>
-      <c r="Q19" s="5"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="5"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="5"/>
+      <c r="Q19" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="R19" s="30"/>
+      <c r="S19" s="30"/>
+      <c r="T19" s="30"/>
+      <c r="U19" s="30"/>
+      <c r="V19" s="30"/>
+      <c r="W19" s="30"/>
       <c r="X19" s="6"/>
       <c r="Y19" s="5"/>
       <c r="Z19" s="6"/>
@@ -1657,7 +1823,9 @@
       <c r="AB19" s="6"/>
       <c r="AC19" s="5"/>
       <c r="AD19" s="6"/>
-      <c r="AE19" s="20"/>
+      <c r="AE19" s="32" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="20" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19"/>
@@ -1917,6 +2085,16 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="R15:V15"/>
+    <mergeCell ref="T18:W18"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="J14:S14"/>
+    <mergeCell ref="H11:N11"/>
+    <mergeCell ref="Q19:W19"/>
+    <mergeCell ref="H12:W12"/>
     <mergeCell ref="C8:G8"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="AE4:AE7"/>
@@ -1926,23 +2104,18 @@
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="J4:P4"/>
     <mergeCell ref="Q4:W4"/>
-    <mergeCell ref="R15:V15"/>
-    <mergeCell ref="Q16:S16"/>
-    <mergeCell ref="T18:W18"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="M17:R17"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="J14:S14"/>
-    <mergeCell ref="H11:N11"/>
-    <mergeCell ref="H12:N12"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>C$7=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="9">
+  <conditionalFormatting sqref="AE1:AE1048576">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"Dokončeno"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="9">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Create a Project Timeline in this worksheet. Enter Start Date in cell C2 and other details starting in cell B4" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in cell at right" sqref="B2" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter Start Date in this cell" sqref="C2:E2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>

</xml_diff>

<commit_message>
Bug fixy, přejmenování, jasnější logika, dokumentace
</commit_message>
<xml_diff>
--- a/timeline/1M Project Timeline.xlsx
+++ b/timeline/1M Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE98F860-6364-42FE-A3F5-54A127098CEE}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DA86CE-47D4-41F1-A028-FB8AB7EF7D6F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -284,7 +284,7 @@
     <t>Daemon druhy backapů</t>
   </si>
   <si>
-    <t>Admin permise</t>
+    <t>Admin permise + víc</t>
   </si>
 </sst>
 </file>
@@ -896,8 +896,8 @@
   </sheetPr>
   <dimension ref="B1:AF27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AA28" sqref="AA28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE22" sqref="AE22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1834,14 +1834,18 @@
       <c r="U20" s="5"/>
       <c r="V20" s="6"/>
       <c r="W20" s="5"/>
-      <c r="X20" s="6"/>
-      <c r="Y20" s="5"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="5"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="5"/>
+      <c r="X20" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+      <c r="AA20" s="23"/>
+      <c r="AB20" s="23"/>
+      <c r="AC20" s="23"/>
       <c r="AD20" s="6"/>
-      <c r="AE20" s="20"/>
+      <c r="AE20" s="22" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="21" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
@@ -1868,14 +1872,18 @@
       <c r="U21" s="5"/>
       <c r="V21" s="6"/>
       <c r="W21" s="5"/>
-      <c r="X21" s="6"/>
-      <c r="Y21" s="5"/>
-      <c r="Z21" s="6"/>
-      <c r="AA21" s="5"/>
-      <c r="AB21" s="6"/>
-      <c r="AC21" s="5"/>
-      <c r="AD21" s="6"/>
-      <c r="AE21" s="20"/>
+      <c r="X21" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="Y21" s="26"/>
+      <c r="Z21" s="26"/>
+      <c r="AA21" s="26"/>
+      <c r="AB21" s="26"/>
+      <c r="AC21" s="26"/>
+      <c r="AD21" s="26"/>
+      <c r="AE21" s="22" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="22" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
@@ -1911,7 +1919,9 @@
       <c r="AB22" s="25"/>
       <c r="AC22" s="25"/>
       <c r="AD22" s="25"/>
-      <c r="AE22" s="20"/>
+      <c r="AE22" s="22" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B23" s="18"/>
@@ -2074,8 +2084,10 @@
       <c r="AE27" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="22">
     <mergeCell ref="X22:AD22"/>
+    <mergeCell ref="X20:AC20"/>
+    <mergeCell ref="X21:AD21"/>
     <mergeCell ref="B1:AE1"/>
     <mergeCell ref="X4:AD4"/>
     <mergeCell ref="C2:E2"/>

</xml_diff>

<commit_message>
Regenerován model. daemon fetchuje tasky. messenger status code fix. Util nova funkce pro Newline, Taskhandler už zpouští akce které dostane
</commit_message>
<xml_diff>
--- a/timeline/1M Project Timeline.xlsx
+++ b/timeline/1M Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DA86CE-47D4-41F1-A028-FB8AB7EF7D6F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F399B8-8FC1-4DDB-AF01-7FEF987F7655}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,7 +149,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Předáno Rambovi.
+Udělám s Rambem.
 Druhy backapů byli přidány do DB</t>
         </r>
       </text>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Druhy backapů</t>
   </si>
   <si>
-    <t>Daemon tasky</t>
-  </si>
-  <si>
     <t>HTTPS</t>
   </si>
   <si>
@@ -263,18 +260,12 @@
     <t>Dokončeno</t>
   </si>
   <si>
-    <t>Nezačnuto</t>
-  </si>
-  <si>
     <t>Probíha</t>
   </si>
   <si>
     <t>Odloženo</t>
   </si>
   <si>
-    <t>Jiné</t>
-  </si>
-  <si>
     <t>Přeloženo</t>
   </si>
   <si>
@@ -285,6 +276,12 @@
   </si>
   <si>
     <t>Admin permise + víc</t>
+  </si>
+  <si>
+    <t>Server tasky</t>
+  </si>
+  <si>
+    <t>???</t>
   </si>
 </sst>
 </file>
@@ -607,35 +604,35 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="10" applyFont="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="11">
@@ -897,7 +894,7 @@
   <dimension ref="B1:AF27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE22" sqref="AE22"/>
+      <selection activeCell="AG21" sqref="AG21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -911,91 +908,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="31">
+      <c r="C2" s="28">
         <v>43143</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="32"/>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="30" t="s">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="32" t="s">
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="30" t="s">
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="27" t="s">
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="27"/>
+      <c r="AE4" s="31" t="s">
         <v>7</v>
       </c>
       <c r="AF4" t="s">
@@ -1116,7 +1113,7 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AE5" s="27"/>
+      <c r="AE5" s="31"/>
       <c r="AF5" t="s">
         <v>6</v>
       </c>
@@ -1235,7 +1232,7 @@
         <f t="shared" si="1"/>
         <v>sun</v>
       </c>
-      <c r="AE6" s="27"/>
+      <c r="AE6" s="31"/>
     </row>
     <row r="7" spans="2:32" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
@@ -1353,19 +1350,19 @@
         <f t="shared" ref="AD7" si="5">AC7+1</f>
         <v>43170</v>
       </c>
-      <c r="AE7" s="28"/>
+      <c r="AE7" s="32"/>
     </row>
     <row r="8" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="24"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="6"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
@@ -1390,20 +1387,20 @@
       <c r="AC8" s="5"/>
       <c r="AD8" s="6"/>
       <c r="AE8" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="6"/>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
@@ -1428,7 +1425,7 @@
       <c r="AC9" s="5"/>
       <c r="AD9" s="6"/>
       <c r="AE9" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1440,14 +1437,14 @@
       <c r="E10" s="5"/>
       <c r="F10" s="6"/>
       <c r="G10" s="5"/>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
       <c r="O10" s="5"/>
       <c r="P10" s="6"/>
       <c r="Q10" s="5"/>
@@ -1465,7 +1462,7 @@
       <c r="AC10" s="5"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="22" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1477,15 +1474,15 @@
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="5"/>
@@ -1503,7 +1500,7 @@
       <c r="AC11" s="5"/>
       <c r="AD11" s="6"/>
       <c r="AE11" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1515,24 +1512,24 @@
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="26" t="s">
+      <c r="H12" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
-      <c r="Q12" s="26"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="26"/>
-      <c r="T12" s="26"/>
-      <c r="U12" s="26"/>
-      <c r="V12" s="26"/>
-      <c r="W12" s="26"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="5"/>
       <c r="Z12" s="6"/>
@@ -1541,7 +1538,7 @@
       <c r="AC12" s="5"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="22" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="2:32" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1557,13 +1554,13 @@
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="6"/>
       <c r="S13" s="5"/>
@@ -1579,12 +1576,12 @@
       <c r="AC13" s="5"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="22" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -1593,18 +1590,18 @@
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="24" t="s">
+      <c r="J14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="24"/>
-      <c r="L14" s="24"/>
-      <c r="M14" s="24"/>
-      <c r="N14" s="24"/>
-      <c r="O14" s="24"/>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="24"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
       <c r="T14" s="6"/>
       <c r="U14" s="5"/>
       <c r="V14" s="6"/>
@@ -1617,12 +1614,12 @@
       <c r="AC14" s="5"/>
       <c r="AD14" s="6"/>
       <c r="AE14" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="6"/>
@@ -1639,13 +1636,13 @@
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="23" t="s">
+      <c r="R15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="S15" s="23"/>
-      <c r="T15" s="23"/>
-      <c r="U15" s="23"/>
-      <c r="V15" s="23"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
       <c r="W15" s="21"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="5"/>
@@ -1655,23 +1652,23 @@
       <c r="AC15" s="5"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="22" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="6"/>
       <c r="E16" s="5"/>
       <c r="F16" s="6"/>
       <c r="G16" s="5"/>
-      <c r="H16" s="25" t="s">
+      <c r="H16" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
       <c r="K16" s="5"/>
       <c r="L16" s="6"/>
       <c r="M16" s="5"/>
@@ -1692,12 +1689,12 @@
       <c r="AC16" s="5"/>
       <c r="AD16" s="6"/>
       <c r="AE16" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="2:31" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B17" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="6"/>
@@ -1709,14 +1706,14 @@
       <c r="J17" s="6"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="26" t="s">
+      <c r="M17" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
       <c r="U17" s="5"/>
@@ -1730,12 +1727,12 @@
       <c r="AC17" s="5"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="22" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="6"/>
@@ -1754,12 +1751,12 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="6"/>
       <c r="S18" s="5"/>
-      <c r="T18" s="24" t="s">
+      <c r="T18" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="U18" s="24"/>
-      <c r="V18" s="24"/>
-      <c r="W18" s="24"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="6"/>
@@ -1768,12 +1765,12 @@
       <c r="AC18" s="5"/>
       <c r="AD18" s="6"/>
       <c r="AE18" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="6"/>
@@ -1789,15 +1786,15 @@
       <c r="N19" s="6"/>
       <c r="O19" s="5"/>
       <c r="P19" s="6"/>
-      <c r="Q19" s="25" t="s">
+      <c r="Q19" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="R19" s="25"/>
-      <c r="S19" s="25"/>
-      <c r="T19" s="25"/>
-      <c r="U19" s="25"/>
-      <c r="V19" s="25"/>
-      <c r="W19" s="25"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
       <c r="X19" s="6"/>
       <c r="Y19" s="5"/>
       <c r="Z19" s="6"/>
@@ -1806,12 +1803,12 @@
       <c r="AC19" s="5"/>
       <c r="AD19" s="6"/>
       <c r="AE19" s="22" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1834,22 +1831,22 @@
       <c r="U20" s="5"/>
       <c r="V20" s="6"/>
       <c r="W20" s="5"/>
-      <c r="X20" s="23" t="s">
+      <c r="X20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="Y20" s="23"/>
-      <c r="Z20" s="23"/>
-      <c r="AA20" s="23"/>
-      <c r="AB20" s="23"/>
-      <c r="AC20" s="23"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="24"/>
       <c r="AD20" s="6"/>
       <c r="AE20" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1872,22 +1869,22 @@
       <c r="U21" s="5"/>
       <c r="V21" s="6"/>
       <c r="W21" s="5"/>
-      <c r="X21" s="26" t="s">
+      <c r="X21" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Y21" s="26"/>
-      <c r="Z21" s="26"/>
-      <c r="AA21" s="26"/>
-      <c r="AB21" s="26"/>
-      <c r="AC21" s="26"/>
-      <c r="AD21" s="26"/>
+      <c r="Y21" s="25"/>
+      <c r="Z21" s="25"/>
+      <c r="AA21" s="25"/>
+      <c r="AB21" s="25"/>
+      <c r="AC21" s="25"/>
+      <c r="AD21" s="25"/>
       <c r="AE21" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
@@ -1910,17 +1907,17 @@
       <c r="U22" s="7"/>
       <c r="V22" s="8"/>
       <c r="W22" s="7"/>
-      <c r="X22" s="25" t="s">
+      <c r="X22" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="Y22" s="25"/>
-      <c r="Z22" s="25"/>
-      <c r="AA22" s="25"/>
-      <c r="AB22" s="25"/>
-      <c r="AC22" s="25"/>
-      <c r="AD22" s="25"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+      <c r="AA22" s="23"/>
+      <c r="AB22" s="23"/>
+      <c r="AC22" s="23"/>
+      <c r="AD22" s="23"/>
       <c r="AE22" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2085,6 +2082,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="J14:S14"/>
+    <mergeCell ref="H11:N11"/>
     <mergeCell ref="X22:AD22"/>
     <mergeCell ref="X20:AC20"/>
     <mergeCell ref="X21:AD21"/>
@@ -2101,12 +2104,6 @@
     <mergeCell ref="AE4:AE7"/>
     <mergeCell ref="R15:V15"/>
     <mergeCell ref="T18:W18"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="M17:R17"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="J14:S14"/>
-    <mergeCell ref="H11:N11"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="1" priority="4">

</xml_diff>

<commit_message>
Upraveno TimedBackups.cs, lepší debugování, vytuněný AdminLogin PasswordFactory umí sha1, upravena M1 timelajna
</commit_message>
<xml_diff>
--- a/timeline/1M Project Timeline.xlsx
+++ b/timeline/1M Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F399B8-8FC1-4DDB-AF01-7FEF987F7655}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E157DD-BFE1-418A-B656-E58657EBDBFD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>Dokončeno</t>
-  </si>
-  <si>
-    <t>Probíha</t>
   </si>
   <si>
     <t>Odloženo</t>
@@ -607,10 +604,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -624,9 +624,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -893,8 +890,8 @@
   </sheetPr>
   <dimension ref="B1:AF27"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AG21" sqref="AG21"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE23" sqref="AE23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -908,90 +905,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26"/>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26"/>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26"/>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26"/>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26"/>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26"/>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26"/>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26"/>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+      <c r="T1" s="27"/>
+      <c r="U1" s="27"/>
+      <c r="V1" s="27"/>
+      <c r="W1" s="27"/>
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27"/>
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="29">
         <v>43143</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="29" t="s">
+      <c r="C4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="29"/>
-      <c r="E4" s="29"/>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="27" t="s">
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="30"/>
+      <c r="G4" s="30"/>
+      <c r="H4" s="30"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="27"/>
-      <c r="L4" s="27"/>
-      <c r="M4" s="27"/>
-      <c r="N4" s="27"/>
-      <c r="O4" s="27"/>
-      <c r="P4" s="27"/>
-      <c r="Q4" s="29" t="s">
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="28"/>
+      <c r="Q4" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="27" t="s">
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="27"/>
-      <c r="Z4" s="27"/>
-      <c r="AA4" s="27"/>
-      <c r="AB4" s="27"/>
-      <c r="AC4" s="27"/>
-      <c r="AD4" s="27"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
+      <c r="AC4" s="28"/>
+      <c r="AD4" s="28"/>
       <c r="AE4" s="31" t="s">
         <v>7</v>
       </c>
@@ -1356,13 +1353,13 @@
       <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="30" t="s">
+      <c r="C8" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
       <c r="H8" s="6"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
@@ -1394,13 +1391,13 @@
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
       <c r="H9" s="6"/>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
@@ -1462,7 +1459,7 @@
       <c r="AC10" s="5"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1474,15 +1471,15 @@
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
-      <c r="L11" s="24"/>
-      <c r="M11" s="24"/>
-      <c r="N11" s="24"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="5"/>
@@ -1512,24 +1509,24 @@
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="O12" s="25"/>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="25"/>
-      <c r="W12" s="25"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24"/>
+      <c r="M12" s="24"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="24"/>
+      <c r="P12" s="24"/>
+      <c r="Q12" s="24"/>
+      <c r="R12" s="24"/>
+      <c r="S12" s="24"/>
+      <c r="T12" s="24"/>
+      <c r="U12" s="24"/>
+      <c r="V12" s="24"/>
+      <c r="W12" s="24"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="5"/>
       <c r="Z12" s="6"/>
@@ -1538,7 +1535,7 @@
       <c r="AC12" s="5"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="2:32" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1554,13 +1551,13 @@
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="24" t="s">
+      <c r="L13" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
+      <c r="M13" s="25"/>
+      <c r="N13" s="25"/>
+      <c r="O13" s="25"/>
+      <c r="P13" s="25"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="6"/>
       <c r="S13" s="5"/>
@@ -1576,12 +1573,12 @@
       <c r="AC13" s="5"/>
       <c r="AD13" s="6"/>
       <c r="AE13" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -1590,18 +1587,18 @@
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="30" t="s">
+      <c r="J14" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="30"/>
-      <c r="N14" s="30"/>
-      <c r="O14" s="30"/>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="30"/>
-      <c r="S14" s="30"/>
+      <c r="K14" s="26"/>
+      <c r="L14" s="26"/>
+      <c r="M14" s="26"/>
+      <c r="N14" s="26"/>
+      <c r="O14" s="26"/>
+      <c r="P14" s="26"/>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="26"/>
+      <c r="S14" s="26"/>
       <c r="T14" s="6"/>
       <c r="U14" s="5"/>
       <c r="V14" s="6"/>
@@ -1636,13 +1633,13 @@
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="24" t="s">
+      <c r="R15" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="24"/>
-      <c r="V15" s="24"/>
+      <c r="S15" s="25"/>
+      <c r="T15" s="25"/>
+      <c r="U15" s="25"/>
+      <c r="V15" s="25"/>
       <c r="W15" s="21"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="5"/>
@@ -1652,7 +1649,7 @@
       <c r="AC15" s="5"/>
       <c r="AD15" s="6"/>
       <c r="AE15" s="22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1706,14 +1703,14 @@
       <c r="J17" s="6"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="25" t="s">
+      <c r="M17" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="N17" s="25"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="25"/>
-      <c r="Q17" s="25"/>
-      <c r="R17" s="25"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
       <c r="U17" s="5"/>
@@ -1727,7 +1724,7 @@
       <c r="AC17" s="5"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1751,12 +1748,12 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="6"/>
       <c r="S18" s="5"/>
-      <c r="T18" s="30" t="s">
+      <c r="T18" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="U18" s="30"/>
-      <c r="V18" s="30"/>
-      <c r="W18" s="30"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="W18" s="26"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="6"/>
@@ -1808,7 +1805,7 @@
     </row>
     <row r="20" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1831,22 +1828,22 @@
       <c r="U20" s="5"/>
       <c r="V20" s="6"/>
       <c r="W20" s="5"/>
-      <c r="X20" s="24" t="s">
+      <c r="X20" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="Y20" s="24"/>
-      <c r="Z20" s="24"/>
-      <c r="AA20" s="24"/>
-      <c r="AB20" s="24"/>
-      <c r="AC20" s="24"/>
+      <c r="Y20" s="25"/>
+      <c r="Z20" s="25"/>
+      <c r="AA20" s="25"/>
+      <c r="AB20" s="25"/>
+      <c r="AC20" s="25"/>
       <c r="AD20" s="6"/>
       <c r="AE20" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1869,22 +1866,22 @@
       <c r="U21" s="5"/>
       <c r="V21" s="6"/>
       <c r="W21" s="5"/>
-      <c r="X21" s="25" t="s">
+      <c r="X21" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="Y21" s="25"/>
-      <c r="Z21" s="25"/>
-      <c r="AA21" s="25"/>
-      <c r="AB21" s="25"/>
-      <c r="AC21" s="25"/>
-      <c r="AD21" s="25"/>
+      <c r="Y21" s="24"/>
+      <c r="Z21" s="24"/>
+      <c r="AA21" s="24"/>
+      <c r="AB21" s="24"/>
+      <c r="AC21" s="24"/>
+      <c r="AD21" s="24"/>
       <c r="AE21" s="22" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
@@ -1917,7 +1914,7 @@
       <c r="AC22" s="23"/>
       <c r="AD22" s="23"/>
       <c r="AE22" s="22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -2082,12 +2079,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="M17:R17"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="J14:S14"/>
-    <mergeCell ref="H11:N11"/>
     <mergeCell ref="X22:AD22"/>
     <mergeCell ref="X20:AC20"/>
     <mergeCell ref="X21:AD21"/>
@@ -2104,6 +2095,12 @@
     <mergeCell ref="AE4:AE7"/>
     <mergeCell ref="R15:V15"/>
     <mergeCell ref="T18:W18"/>
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="J14:S14"/>
+    <mergeCell ref="H11:N11"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="1" priority="4">

</xml_diff>

<commit_message>
Zlepšení db, už se odesílají informace o tom jak se má zipovat
</commit_message>
<xml_diff>
--- a/timeline/1M Project Timeline.xlsx
+++ b/timeline/1M Project Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\Programming\Workspace\C#\Backupper\timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E157DD-BFE1-418A-B656-E58657EBDBFD}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E1984B-B4AB-483C-ABA3-5D6C759C12F6}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,31 +129,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="AE13" authorId="0" shapeId="0" xr:uid="{F7C1B304-9226-4C83-875A-82D396B247D1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>lukx:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Udělám s Rambem.
-Druhy backapů byli přidány do DB</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="B19" authorId="0" shapeId="0" xr:uid="{FE1D2AA7-EA35-473E-9EDB-FAD401627DB4}">
       <text>
         <r>
@@ -183,7 +158,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>4 week project timeline</t>
   </si>
@@ -263,9 +238,6 @@
     <t>Odloženo</t>
   </si>
   <si>
-    <t>Přeloženo</t>
-  </si>
-  <si>
     <t>Daemon načítání tasků a timery</t>
   </si>
   <si>
@@ -278,7 +250,7 @@
     <t>Server tasky</t>
   </si>
   <si>
-    <t>???</t>
+    <t>Nedokončeno</t>
   </si>
 </sst>
 </file>
@@ -604,26 +576,26 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="4" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="6">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
@@ -891,7 +863,7 @@
   <dimension ref="B1:AF27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE23" sqref="AE23"/>
+      <selection activeCell="AF10" sqref="AF10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -905,90 +877,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:32" ht="48.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
-      <c r="Y1" s="27"/>
-      <c r="Z1" s="27"/>
-      <c r="AA1" s="27"/>
-      <c r="AB1" s="27"/>
-      <c r="AC1" s="27"/>
-      <c r="AD1" s="27"/>
-      <c r="AE1" s="27"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26"/>
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26"/>
     </row>
     <row r="2" spans="2:32" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="29">
+      <c r="C2" s="28">
         <v>43143</v>
       </c>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
     </row>
     <row r="3" spans="2:32" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="2:32" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="9"/>
-      <c r="C4" s="30" t="s">
+      <c r="C4" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30"/>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="28" t="s">
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="30" t="s">
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
+      <c r="Q4" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="30"/>
-      <c r="X4" s="28" t="s">
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="29"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="Y4" s="28"/>
-      <c r="Z4" s="28"/>
-      <c r="AA4" s="28"/>
-      <c r="AB4" s="28"/>
-      <c r="AC4" s="28"/>
-      <c r="AD4" s="28"/>
+      <c r="Y4" s="27"/>
+      <c r="Z4" s="27"/>
+      <c r="AA4" s="27"/>
+      <c r="AB4" s="27"/>
+      <c r="AC4" s="27"/>
+      <c r="AD4" s="27"/>
       <c r="AE4" s="31" t="s">
         <v>7</v>
       </c>
@@ -1353,13 +1325,13 @@
       <c r="B8" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
       <c r="H8" s="6"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
@@ -1391,13 +1363,13 @@
       <c r="B9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="6"/>
       <c r="I9" s="5"/>
       <c r="J9" s="6"/>
@@ -1459,7 +1431,7 @@
       <c r="AC10" s="5"/>
       <c r="AD10" s="6"/>
       <c r="AE10" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1471,15 +1443,15 @@
       <c r="E11" s="5"/>
       <c r="F11" s="6"/>
       <c r="G11" s="5"/>
-      <c r="H11" s="25" t="s">
+      <c r="H11" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24"/>
+      <c r="M11" s="24"/>
+      <c r="N11" s="24"/>
       <c r="O11" s="5"/>
       <c r="P11" s="6"/>
       <c r="Q11" s="5"/>
@@ -1509,24 +1481,24 @@
       <c r="E12" s="5"/>
       <c r="F12" s="6"/>
       <c r="G12" s="5"/>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="24"/>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="24"/>
-      <c r="S12" s="24"/>
-      <c r="T12" s="24"/>
-      <c r="U12" s="24"/>
-      <c r="V12" s="24"/>
-      <c r="W12" s="24"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="25"/>
+      <c r="Q12" s="25"/>
+      <c r="R12" s="25"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="25"/>
+      <c r="U12" s="25"/>
+      <c r="V12" s="25"/>
+      <c r="W12" s="25"/>
       <c r="X12" s="6"/>
       <c r="Y12" s="5"/>
       <c r="Z12" s="6"/>
@@ -1535,7 +1507,7 @@
       <c r="AC12" s="5"/>
       <c r="AD12" s="6"/>
       <c r="AE12" s="22" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="2:32" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -1551,13 +1523,13 @@
       <c r="I13" s="5"/>
       <c r="J13" s="6"/>
       <c r="K13" s="5"/>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="M13" s="25"/>
-      <c r="N13" s="25"/>
-      <c r="O13" s="25"/>
-      <c r="P13" s="25"/>
+      <c r="M13" s="24"/>
+      <c r="N13" s="24"/>
+      <c r="O13" s="24"/>
+      <c r="P13" s="24"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="6"/>
       <c r="S13" s="5"/>
@@ -1578,7 +1550,7 @@
     </row>
     <row r="14" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C14" s="5"/>
       <c r="D14" s="6"/>
@@ -1587,18 +1559,18 @@
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
       <c r="I14" s="5"/>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="30"/>
+      <c r="O14" s="30"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="30"/>
       <c r="T14" s="6"/>
       <c r="U14" s="5"/>
       <c r="V14" s="6"/>
@@ -1633,13 +1605,13 @@
       <c r="O15" s="5"/>
       <c r="P15" s="6"/>
       <c r="Q15" s="5"/>
-      <c r="R15" s="25" t="s">
+      <c r="R15" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="25"/>
+      <c r="S15" s="24"/>
+      <c r="T15" s="24"/>
+      <c r="U15" s="24"/>
+      <c r="V15" s="24"/>
       <c r="W15" s="21"/>
       <c r="X15" s="6"/>
       <c r="Y15" s="5"/>
@@ -1703,14 +1675,14 @@
       <c r="J17" s="6"/>
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
-      <c r="M17" s="24" t="s">
+      <c r="M17" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
       <c r="S17" s="5"/>
       <c r="T17" s="6"/>
       <c r="U17" s="5"/>
@@ -1724,7 +1696,7 @@
       <c r="AC17" s="5"/>
       <c r="AD17" s="6"/>
       <c r="AE17" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
@@ -1748,12 +1720,12 @@
       <c r="Q18" s="5"/>
       <c r="R18" s="6"/>
       <c r="S18" s="5"/>
-      <c r="T18" s="26" t="s">
+      <c r="T18" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
+      <c r="U18" s="30"/>
+      <c r="V18" s="30"/>
+      <c r="W18" s="30"/>
       <c r="X18" s="6"/>
       <c r="Y18" s="5"/>
       <c r="Z18" s="6"/>
@@ -1805,7 +1777,7 @@
     </row>
     <row r="20" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="6"/>
@@ -1828,14 +1800,14 @@
       <c r="U20" s="5"/>
       <c r="V20" s="6"/>
       <c r="W20" s="5"/>
-      <c r="X20" s="25" t="s">
+      <c r="X20" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="Y20" s="25"/>
-      <c r="Z20" s="25"/>
-      <c r="AA20" s="25"/>
-      <c r="AB20" s="25"/>
-      <c r="AC20" s="25"/>
+      <c r="Y20" s="24"/>
+      <c r="Z20" s="24"/>
+      <c r="AA20" s="24"/>
+      <c r="AB20" s="24"/>
+      <c r="AC20" s="24"/>
       <c r="AD20" s="6"/>
       <c r="AE20" s="22" t="s">
         <v>24</v>
@@ -1843,7 +1815,7 @@
     </row>
     <row r="21" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="6"/>
@@ -1866,22 +1838,22 @@
       <c r="U21" s="5"/>
       <c r="V21" s="6"/>
       <c r="W21" s="5"/>
-      <c r="X21" s="24" t="s">
+      <c r="X21" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="Y21" s="24"/>
-      <c r="Z21" s="24"/>
-      <c r="AA21" s="24"/>
-      <c r="AB21" s="24"/>
-      <c r="AC21" s="24"/>
-      <c r="AD21" s="24"/>
+      <c r="Y21" s="25"/>
+      <c r="Z21" s="25"/>
+      <c r="AA21" s="25"/>
+      <c r="AB21" s="25"/>
+      <c r="AC21" s="25"/>
+      <c r="AD21" s="25"/>
       <c r="AE21" s="22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="2:31" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="8"/>
@@ -2079,6 +2051,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="I10:N10"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="L13:P13"/>
+    <mergeCell ref="J14:S14"/>
+    <mergeCell ref="H11:N11"/>
     <mergeCell ref="X22:AD22"/>
     <mergeCell ref="X20:AC20"/>
     <mergeCell ref="X21:AD21"/>
@@ -2095,12 +2073,6 @@
     <mergeCell ref="AE4:AE7"/>
     <mergeCell ref="R15:V15"/>
     <mergeCell ref="T18:W18"/>
-    <mergeCell ref="I10:N10"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="M17:R17"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="J14:S14"/>
-    <mergeCell ref="H11:N11"/>
   </mergeCells>
   <conditionalFormatting sqref="C6:AD7">
     <cfRule type="expression" dxfId="1" priority="4">

</xml_diff>